<commit_message>
Added a Gantt Chart template to week10 of sed200.
</commit_message>
<xml_diff>
--- a/sed200/Week10/CribAssembly.xlsx
+++ b/sed200/Week10/CribAssembly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Seneca\github\MWATLER.github.io\sed200\Week10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9846E194-F45C-4D95-B1B5-FEBE5B89001B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC83BC0F-C0BA-4417-96B1-3AFC2774530A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Activity</t>
   </si>
   <si>
-    <t>duration</t>
-  </si>
-  <si>
     <t>precedence</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>10.Assemble wall 3</t>
   </si>
   <si>
-    <t>Crib Assemble</t>
-  </si>
-  <si>
     <t>2.Assemble baby mobile</t>
   </si>
   <si>
@@ -106,16 +100,30 @@
   </si>
   <si>
     <t>20.Attach wall 4 to base</t>
+  </si>
+  <si>
+    <t>duration (hrs)</t>
+  </si>
+  <si>
+    <t>Crib Assembly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,11 +149,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,143 +438,206 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>1.5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B18">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>26</v>
+      <c r="B23">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>